<commit_message>
client derby et pg ok
</commit_message>
<xml_diff>
--- a/Doc/GZA/Journal_Travail_Guillaume.xlsx
+++ b/Doc/GZA/Journal_Travail_Guillaume.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F723E22-6F9D-4E48-815A-1E26BB852A9B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFF2456-F25F-412D-AB9A-07C4E8037BD7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>rapport</t>
+  </si>
+  <si>
+    <t>développement du crud et test sur ClientRepository et mise en place de la classe ORM</t>
+  </si>
+  <si>
+    <t>développement et test de ClientRepository pour derby</t>
   </si>
 </sst>
 </file>
@@ -223,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -253,6 +259,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +543,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,13 +908,23 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+      <c r="A35" s="15">
+        <v>43204</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
+      <c r="A36" s="15">
+        <v>43204</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="C36" s="13"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -971,7 +988,7 @@
       </c>
       <c r="C48" s="9">
         <f>SUM(C5:C47)</f>
-        <v>31.749999999999996</v>
+        <v>32.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ok id add account
</commit_message>
<xml_diff>
--- a/Doc/GZA/Journal_Travail_Guillaume.xlsx
+++ b/Doc/GZA/Journal_Travail_Guillaume.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFF2456-F25F-412D-AB9A-07C4E8037BD7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2031A3-6BB4-4761-A33C-2BE1BB740FB1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>développement et test de ClientRepository pour derby</t>
+  </si>
+  <si>
+    <t>Problème avec les id généré automatiquement dans derby</t>
   </si>
 </sst>
 </file>
@@ -256,10 +259,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,10 +561,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
@@ -908,7 +911,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="15">
+      <c r="A35" s="14">
         <v>43204</v>
       </c>
       <c r="B35" s="13" t="s">
@@ -919,18 +922,26 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="15">
+      <c r="A36" s="14">
         <v>43204</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="13"/>
+      <c r="C36" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="8"/>
+      <c r="A37" s="11">
+        <v>43204</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
@@ -988,7 +999,7 @@
       </c>
       <c r="C48" s="9">
         <f>SUM(C5:C47)</f>
-        <v>32.25</v>
+        <v>36.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>